<commit_message>
We recovered part of the participant's solution.
The participant's solution was recovered. However, the blocks that were not attached to the starting block of the block-based language were lost.
</commit_message>
<xml_diff>
--- a/Last_Experiment_Post_Experiment_Questionnaire.xlsx
+++ b/Last_Experiment_Post_Experiment_Questionnaire.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conso\OneDrive\Documents\GitHub\robot-barriers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BFE6A6-2DF3-4941-9950-3658C63CB311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="109">
   <si>
     <t>Timestamp</t>
   </si>
@@ -326,14 +335,6 @@
     <t>p04121200</t>
   </si>
   <si>
-    <t>No. The Wizard Easy Programming tool saving feature was not working. The solution made by the participant was lost.</t>
-  </si>
-  <si>
-    <t>The desktop application was not working properly the first time the participant tried to use it. The proctor had to restart the website, losing the hours the participant took to complete the experiment. However, the proctor manually annotated the hours on his phone. The participant took 1 hour and 20 minutes to work on the experiment. No interactions were lost in the process, as this was the first time the participant was using the desktop application. 
-At the time of saving the participant's program solution, the saving feature of the Wizard Easy Program tool was not working properly too. The proctor had to restart the FlexPendant to make the Wizard Easy Programming tool work again, losing the participant's solution from the memory of the computer.
-However, the proctor observed the solution of the participant, and noticed that the participant did not complete the task. About five blocks or placed on the Wizard Easy Programming tool. The participant's solution should be considered incomplete.</t>
-  </si>
-  <si>
     <t>The materials do not provide the sufficient or required information, The information and resources are not concise and clear, The information and resources are not organized into logical and understandable components</t>
   </si>
   <si>
@@ -348,23 +349,28 @@
   </si>
   <si>
     <t>I found it very easy to get the movements down! The complicated part was figuring out the welcome message and movement question. The variables were also difficult to understand and I think providing more material on what they are for will help!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The desktop application was not working properly the first time the participant tried to use it. The proctor had to restart the website, losing the hours the participant took to complete the experiment. However, the proctor manually annotated the hours on his phone. The participant took 1 hour and 20 minutes to work on the experiment. No interactions were lost in the process, as this was the first time the participant was using the desktop application. 
+At the time of saving the participant's program solution, the saving feature of the Wizard Easy Program tool was not working properly, maybe due to many errors in the participant's solution. The proctor had to restart the FlexPendant to make the Wizard Easy Programming tool work again. The participant had blocks that were not attached to the starting block of the tool, and these blocks were lost when we restarted the system. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -375,7 +381,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -385,42 +391,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -610,26 +618,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col customWidth="1" min="1" max="32" width="18.88"/>
+    <col min="1" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="79.44140625" customWidth="1"/>
+    <col min="6" max="32" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,715 +718,715 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2">
         <v>45392.457167430555</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="R2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X2" s="4" t="s">
+      <c r="U2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2">
         <v>45392.5118530787</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="V3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2">
         <v>45392.646322256944</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="T4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="U4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="V4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Y4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="Z4" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3">
-        <v>45392.71231827546</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2">
+        <v>45392.712318275459</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R5" s="4" t="s">
+      <c r="Q5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U5" s="4" t="s">
+      <c r="S5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X5" s="4" t="s">
+      <c r="V5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Y5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="Z5" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2">
         <v>45393.51467798611</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="P6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V6" s="4" t="s">
+      <c r="S6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="W6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="X6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Y6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="Z6" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="3">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
         <v>45393.603960092594</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="4" t="s">
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="Q7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="4" t="s">
+      <c r="Q7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y7" s="4" t="s">
+      <c r="U7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Z7" s="4" t="s">
+      <c r="Z7" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2">
         <v>45393.653702118056</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="4" t="s">
+      <c r="H8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Q8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X8" s="4" t="s">
+      <c r="Q8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="Y8" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="3">
-        <v>45393.71873298611</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2">
+        <v>45393.718732986112</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="S9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="T9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="U9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V9" s="4" t="s">
+      <c r="V9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="X9" s="4" t="s">
+      <c r="X9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Y9" s="4" t="s">
+      <c r="Y9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Z9" s="4" t="s">
+      <c r="Z9" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3">
-        <v>45394.4518971412</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2">
+        <v>45394.451897141204</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="H10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="S10" s="4" t="s">
+      <c r="Q10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="T10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U10" s="4" t="s">
+      <c r="U10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="V10" s="4" t="s">
+      <c r="V10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="X10" s="4" t="s">
+      <c r="X10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z10" s="4" t="s">
+      <c r="Z10" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3">
-        <v>45394.51732225694</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2">
+        <v>45394.517322256943</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="O11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L11" s="4" t="s">
+      <c r="Q11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="O11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" s="4" t="s">
+      <c r="Y11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="Q11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W11" s="4" t="s">
+      <c r="Z11" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>